<commit_message>
fix: figure label cutting off
</commit_message>
<xml_diff>
--- a/outputs/survey_profiles.xlsx
+++ b/outputs/survey_profiles.xlsx
@@ -501,23 +501,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bachelor’s degree</t>
+          <t>Other (please specify below)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>12.9</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="4">
@@ -555,23 +555,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Other (please specify below)</t>
+          <t>Bachelor’s degree</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
-        <v>3.2</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="6">
@@ -582,11 +582,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Industry</t>
+          <t>Government</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -595,10 +595,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>6.5</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="7">
@@ -609,11 +609,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Government</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -622,10 +622,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>3.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="8">
@@ -663,23 +663,23 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Undergraduate student</t>
+          <t>Graduate student (including professional school student)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>3.2</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="10">
@@ -690,23 +690,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Faculty member</t>
+          <t>Undergraduate student</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>32.3</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="11">
@@ -717,23 +717,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Staff member (including research/academic/teaching staff)</t>
+          <t>Postdoc</t>
         </is>
       </c>
       <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
         <v>2</v>
       </c>
-      <c r="D11" t="n">
-        <v>5</v>
-      </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G11" t="n">
-        <v>32.3</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="12">
@@ -744,23 +744,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Postdoc</t>
+          <t>Faculty member</t>
         </is>
       </c>
       <c r="C12" t="n">
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G12" t="n">
-        <v>12.9</v>
+        <v>32.3</v>
       </c>
     </row>
     <row r="13">
@@ -798,23 +798,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Graduate student (including professional school student)</t>
+          <t>Staff member (including research/academic/teaching staff)</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G14" t="n">
-        <v>12.9</v>
+        <v>32.3</v>
       </c>
     </row>
     <row r="15">

</xml_diff>

<commit_message>
fix: rerun survey notebook
</commit_message>
<xml_diff>
--- a/outputs/survey_profiles.xlsx
+++ b/outputs/survey_profiles.xlsx
@@ -501,23 +501,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Graduate or professional degree (MA, MS, MBA, PhD, JD, MD, DDS etc.)</t>
+          <t>Bachelor’s degree</t>
         </is>
       </c>
       <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
         <v>4</v>
       </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>82.8</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="4">
@@ -528,23 +528,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bachelor’s degree</t>
+          <t>Graduate or professional degree (MA, MS, MBA, PhD, JD, MD, DDS etc.)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="G4" t="n">
-        <v>13.8</v>
+        <v>82.8</v>
       </c>
     </row>
     <row r="5">
@@ -609,23 +609,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Industry</t>
+          <t>Academia</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="G7" t="n">
-        <v>6.9</v>
+        <v>89.7</v>
       </c>
     </row>
     <row r="8">
@@ -636,23 +636,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Academia</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>89.7</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="9">
@@ -663,23 +663,23 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Other (please specify below)</t>
+          <t>Postdoc</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>6.9</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="10">
@@ -690,23 +690,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Postdoc</t>
+          <t>Staff member (including research/academic/teaching staff)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G10" t="n">
-        <v>13.8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -717,23 +717,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Undergraduate student</t>
+          <t>Graduate student (including professional school student)</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11" t="n">
-        <v>3.4</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="12">
@@ -744,23 +744,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Staff member (including research/academic/teaching staff)</t>
+          <t>Other (please specify below)</t>
         </is>
       </c>
       <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
         <v>2</v>
       </c>
-      <c r="D12" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" t="n">
-        <v>3</v>
-      </c>
-      <c r="F12" t="n">
-        <v>9</v>
-      </c>
       <c r="G12" t="n">
-        <v>31</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="13">
@@ -771,23 +771,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Graduate student (including professional school student)</t>
+          <t>Faculty member</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G13" t="n">
-        <v>13.8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
@@ -798,23 +798,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Faculty member</t>
+          <t>Undergraduate student</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>31</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="15">
@@ -825,23 +825,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>More than 5 years</t>
+          <t>Less than 1 year</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
         <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G15" t="n">
-        <v>31</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="16">
@@ -852,23 +852,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Less than 1 year</t>
+          <t>1 to 5 years</t>
         </is>
       </c>
       <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E16" t="n">
         <v>3</v>
       </c>
-      <c r="D16" t="n">
-        <v>2</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
       <c r="F16" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G16" t="n">
-        <v>17.2</v>
+        <v>51.7</v>
       </c>
     </row>
     <row r="17">
@@ -879,23 +879,23 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1 to 5 years</t>
+          <t>More than 5 years</t>
         </is>
       </c>
       <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
         <v>2</v>
       </c>
-      <c r="D17" t="n">
-        <v>10</v>
-      </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G17" t="n">
-        <v>51.7</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>